<commit_message>
Follow up post planting!
</commit_message>
<xml_diff>
--- a/Planning/Inds for Planting Final.six.xlsx
+++ b/Planning/Inds for Planting Final.six.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="13580" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18460" windowHeight="14360" tabRatio="500" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="2 (2)" sheetId="6" r:id="rId1"/>
@@ -873,9 +873,6 @@
     <t>SPITOM_HF_9</t>
   </si>
   <si>
-    <t>SPIALB_GR_4</t>
-  </si>
-  <si>
     <t>SPITOM_HF_13</t>
   </si>
   <si>
@@ -946,6 +943,9 @@
   </si>
   <si>
     <t>(was ALNINC_GR_1)</t>
+  </si>
+  <si>
+    <t>ACESPI_SH_9</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1058,7 @@
       <name val="Zapf Dingbats"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1092,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1433,7 +1445,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1203">
+  <cellStyleXfs count="1209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2637,8 +2649,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2988,9 +3006,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3080,17 +3095,38 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1203">
+  <cellStyles count="1209">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3692,6 +3728,9 @@
     <cellStyle name="Followed Hyperlink" xfId="1198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1208" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4293,6 +4332,9 @@
     <cellStyle name="Hyperlink" xfId="1197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1207" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6064,8 +6106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="G7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView topLeftCell="C20" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -6537,8 +6579,8 @@
       <c r="H14" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="137" t="s">
-        <v>295</v>
+      <c r="I14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
@@ -6563,12 +6605,12 @@
       <c r="X14" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="Y14" s="137" t="s">
-        <v>295</v>
+      <c r="Y14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="Z14" s="24"/>
       <c r="AA14" s="26"/>
-      <c r="AB14" s="24" t="s">
+      <c r="AB14" s="164" t="s">
         <v>41</v>
       </c>
       <c r="AC14" s="24"/>
@@ -6577,8 +6619,8 @@
       <c r="AF14" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="AG14" s="148" t="s">
-        <v>295</v>
+      <c r="AG14" s="147" t="s">
+        <v>294</v>
       </c>
       <c r="AH14" s="5"/>
       <c r="AI14" s="6"/>
@@ -6880,7 +6922,7 @@
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
       <c r="O22" s="26"/>
-      <c r="P22" s="24" t="s">
+      <c r="P22" s="164" t="s">
         <v>63</v>
       </c>
       <c r="Q22" s="24"/>
@@ -6904,8 +6946,8 @@
       <c r="AC22" s="24"/>
       <c r="AD22" s="24"/>
       <c r="AE22" s="27"/>
-      <c r="AF22" s="80" t="s">
-        <v>31</v>
+      <c r="AF22" s="128" t="s">
+        <v>257</v>
       </c>
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
@@ -7016,9 +7058,9 @@
       <c r="AB25" s="29"/>
       <c r="AC25" s="29"/>
       <c r="AD25" s="29"/>
-      <c r="AE25" s="130"/>
+      <c r="AE25" s="129"/>
       <c r="AF25" s="103"/>
-      <c r="AG25" s="133"/>
+      <c r="AG25" s="132"/>
       <c r="AH25" s="5"/>
       <c r="AI25" s="6"/>
     </row>
@@ -7032,8 +7074,8 @@
       <c r="G26" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="H26" s="88" t="s">
-        <v>278</v>
+      <c r="H26" s="133" t="s">
+        <v>24</v>
       </c>
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
@@ -7047,8 +7089,8 @@
       <c r="P26" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="Q26" s="137" t="s">
-        <v>295</v>
+      <c r="Q26" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="R26" s="24"/>
       <c r="S26" s="24"/>
@@ -7059,7 +7101,7 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
       <c r="X26" s="90" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y26" s="24"/>
       <c r="Z26" s="24"/>
@@ -7067,11 +7109,11 @@
       <c r="AB26" s="24"/>
       <c r="AC26" s="24"/>
       <c r="AD26" s="24"/>
-      <c r="AE26" s="131"/>
+      <c r="AE26" s="130"/>
       <c r="AF26" s="63" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG26" s="133"/>
+        <v>279</v>
+      </c>
+      <c r="AG26" s="132"/>
       <c r="AH26" s="5"/>
       <c r="AI26" s="6"/>
     </row>
@@ -7106,9 +7148,9 @@
       <c r="AB27" s="19"/>
       <c r="AC27" s="19"/>
       <c r="AD27" s="19"/>
-      <c r="AE27" s="132"/>
+      <c r="AE27" s="131"/>
       <c r="AF27" s="103"/>
-      <c r="AG27" s="133"/>
+      <c r="AG27" s="132"/>
       <c r="AH27" s="5"/>
       <c r="AI27" s="6"/>
     </row>
@@ -7196,7 +7238,7 @@
       <c r="G30" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="162" t="s">
         <v>25</v>
       </c>
       <c r="I30" s="19"/>
@@ -7205,8 +7247,8 @@
       <c r="L30" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="M30" s="139" t="s">
-        <v>295</v>
+      <c r="M30" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="N30" s="19"/>
       <c r="O30" s="21"/>
@@ -7237,8 +7279,8 @@
       <c r="AF30" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="AG30" s="148" t="s">
-        <v>295</v>
+      <c r="AG30" s="147" t="s">
+        <v>294</v>
       </c>
       <c r="AH30" s="5"/>
       <c r="AI30" s="6"/>
@@ -7363,7 +7405,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="63" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -7372,7 +7414,7 @@
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
-      <c r="P34" s="19" t="s">
+      <c r="P34" s="64" t="s">
         <v>16</v>
       </c>
       <c r="Q34" s="19"/>
@@ -7528,8 +7570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="H12" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView topLeftCell="D22" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="AE28" sqref="AE28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7840,8 +7882,8 @@
       <c r="H10" s="85" t="s">
         <v>187</v>
       </c>
-      <c r="I10" s="147" t="s">
-        <v>295</v>
+      <c r="I10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -7892,7 +7934,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="20"/>
       <c r="U11" s="63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
@@ -7937,8 +7979,8 @@
       <c r="AA12" s="21"/>
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
-      <c r="AD12" s="129" t="s">
-        <v>297</v>
+      <c r="AD12" s="128" t="s">
+        <v>296</v>
       </c>
       <c r="AE12" s="22"/>
       <c r="AF12" s="19"/>
@@ -8087,8 +8129,8 @@
       <c r="M16" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="N16" s="139" t="s">
-        <v>295</v>
+      <c r="N16" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="O16" s="21"/>
       <c r="P16" s="19"/>
@@ -8136,8 +8178,8 @@
       <c r="U17" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="V17" s="150" t="s">
-        <v>295</v>
+      <c r="V17" s="149" t="s">
+        <v>294</v>
       </c>
       <c r="W17" s="29"/>
       <c r="X17" s="30"/>
@@ -8260,8 +8302,8 @@
       <c r="N20" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="O20" s="156" t="s">
-        <v>295</v>
+      <c r="O20" s="155" t="s">
+        <v>294</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
@@ -8312,8 +8354,8 @@
       <c r="Y21" s="80" t="s">
         <v>188</v>
       </c>
-      <c r="Z21" s="139" t="s">
-        <v>295</v>
+      <c r="Z21" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AA21" s="21"/>
       <c r="AB21" s="19"/>
@@ -8421,7 +8463,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="82" t="s">
+      <c r="H24" s="101" t="s">
         <v>122</v>
       </c>
       <c r="I24" s="19"/>
@@ -8433,7 +8475,7 @@
       <c r="O24" s="21"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
-      <c r="R24" s="129" t="s">
+      <c r="R24" s="128" t="s">
         <v>95</v>
       </c>
       <c r="S24" s="19"/>
@@ -8594,8 +8636,8 @@
       <c r="M28" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="N28" s="139" t="s">
-        <v>295</v>
+      <c r="N28" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="19"/>
@@ -8616,8 +8658,8 @@
       <c r="AE28" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="AF28" s="149" t="s">
-        <v>295</v>
+      <c r="AF28" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG28" s="5"/>
       <c r="AH28" s="5"/>
@@ -8813,7 +8855,7 @@
       <c r="W33" s="34"/>
       <c r="X33" s="35"/>
       <c r="Y33" s="77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Z33" s="34"/>
       <c r="AA33" s="36"/>
@@ -9005,8 +9047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="D11" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -9328,7 +9370,7 @@
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -9337,7 +9379,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
       <c r="AA10" s="16"/>
-      <c r="AB10" s="79" t="s">
+      <c r="AB10" s="97" t="s">
         <v>136</v>
       </c>
       <c r="AC10" s="13"/>
@@ -9373,7 +9415,7 @@
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
       <c r="X11" s="71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y11" s="19"/>
       <c r="Z11" s="19"/>
@@ -9477,7 +9519,7 @@
         <v>202</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="26"/>
@@ -9578,7 +9620,7 @@
       <c r="Y16" s="19"/>
       <c r="Z16" s="19"/>
       <c r="AA16" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AB16" s="19"/>
       <c r="AC16" s="19"/>
@@ -9710,15 +9752,15 @@
       <c r="W19" s="19"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="19"/>
-      <c r="Z19" s="80" t="s">
-        <v>136</v>
+      <c r="Z19" s="128" t="s">
+        <v>302</v>
       </c>
       <c r="AA19" s="21"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
-      <c r="AE19" s="143" t="s">
-        <v>298</v>
+      <c r="AE19" s="142" t="s">
+        <v>297</v>
       </c>
       <c r="AF19" s="41"/>
       <c r="AG19" s="5"/>
@@ -9836,7 +9878,7 @@
       </c>
       <c r="Y22" s="24"/>
       <c r="Z22" s="24"/>
-      <c r="AA22" s="62" t="s">
+      <c r="AA22" s="160" t="s">
         <v>264</v>
       </c>
       <c r="AB22" s="44" t="s">
@@ -9871,8 +9913,8 @@
       <c r="N23" s="19"/>
       <c r="O23" s="21"/>
       <c r="P23" s="19"/>
-      <c r="Q23" s="129" t="s">
-        <v>298</v>
+      <c r="Q23" s="128" t="s">
+        <v>297</v>
       </c>
       <c r="R23" s="19"/>
       <c r="S23" s="19"/>
@@ -9943,10 +9985,10 @@
       <c r="F25" s="5"/>
       <c r="G25" s="103"/>
       <c r="H25" s="65" t="s">
-        <v>288</v>
-      </c>
-      <c r="I25" s="153" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="I25" s="152" t="s">
+        <v>294</v>
       </c>
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
@@ -9982,7 +10024,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="144" t="s">
+      <c r="G26" s="143" t="s">
         <v>223</v>
       </c>
       <c r="H26" s="98"/>
@@ -10007,7 +10049,7 @@
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
-      <c r="X26" s="127" t="s">
+      <c r="X26" s="166" t="s">
         <v>273</v>
       </c>
       <c r="Y26" s="24"/>
@@ -10040,8 +10082,8 @@
       <c r="K27" s="19"/>
       <c r="L27" s="20"/>
       <c r="M27" s="19"/>
-      <c r="N27" s="129" t="s">
-        <v>298</v>
+      <c r="N27" s="128" t="s">
+        <v>297</v>
       </c>
       <c r="O27" s="21"/>
       <c r="P27" s="19"/>
@@ -10126,7 +10168,7 @@
       <c r="O29" s="31"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S29" s="29"/>
       <c r="T29" s="30"/>
@@ -10177,8 +10219,8 @@
       <c r="W30" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="X30" s="160" t="s">
-        <v>295</v>
+      <c r="X30" s="158" t="s">
+        <v>294</v>
       </c>
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
@@ -10206,7 +10248,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="118" t="s">
+      <c r="H31" s="161" t="s">
         <v>161</v>
       </c>
       <c r="I31" s="19"/>
@@ -10267,8 +10309,8 @@
       <c r="AA32" s="111" t="s">
         <v>152</v>
       </c>
-      <c r="AB32" s="139" t="s">
-        <v>295</v>
+      <c r="AB32" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AC32" s="19"/>
       <c r="AD32" s="19"/>
@@ -10342,7 +10384,7 @@
       <c r="Q34" s="19"/>
       <c r="R34" s="19"/>
       <c r="S34" s="80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T34" s="55"/>
       <c r="U34" s="19"/>
@@ -10360,7 +10402,7 @@
       <c r="AC34" s="19"/>
       <c r="AD34" s="19"/>
       <c r="AE34" s="126" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AF34" s="43" t="s">
         <v>204</v>
@@ -10497,8 +10539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+    <sheetView topLeftCell="G17" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -10822,7 +10864,7 @@
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="119" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -10830,8 +10872,8 @@
       <c r="X10" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="Y10" s="147" t="s">
-        <v>295</v>
+      <c r="Y10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="Z10" s="13"/>
       <c r="AA10" s="16"/>
@@ -11147,19 +11189,19 @@
       <c r="Q18" s="19"/>
       <c r="R18" s="19"/>
       <c r="S18" s="19"/>
-      <c r="T18" s="71" t="s">
+      <c r="T18" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="U18" s="139" t="s">
-        <v>295</v>
+      <c r="U18" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="V18" s="19"/>
       <c r="W18" s="19"/>
       <c r="X18" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="Y18" s="139" t="s">
-        <v>295</v>
+      <c r="Y18" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="Z18" s="19"/>
       <c r="AA18" s="21"/>
@@ -11328,8 +11370,8 @@
       <c r="AB22" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="AC22" s="137" t="s">
-        <v>295</v>
+      <c r="AC22" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="AD22" s="24"/>
       <c r="AE22" s="27"/>
@@ -11956,8 +11998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="G18" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -12278,8 +12320,8 @@
       <c r="S10" s="79" t="s">
         <v>187</v>
       </c>
-      <c r="T10" s="138" t="s">
-        <v>295</v>
+      <c r="T10" s="137" t="s">
+        <v>294</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -12775,7 +12817,7 @@
       </c>
       <c r="Y22" s="24"/>
       <c r="Z22" s="24"/>
-      <c r="AA22" s="128" t="s">
+      <c r="AA22" s="127" t="s">
         <v>73</v>
       </c>
       <c r="AB22" s="44" t="s">
@@ -13412,8 +13454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AL18" sqref="AL18"/>
+    <sheetView topLeftCell="G19" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -13719,10 +13761,10 @@
       <c r="F10" s="5"/>
       <c r="G10" s="19"/>
       <c r="H10" s="85" t="s">
-        <v>288</v>
-      </c>
-      <c r="I10" s="147" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="I10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -13750,10 +13792,10 @@
       <c r="AC10" s="13"/>
       <c r="AD10" s="13"/>
       <c r="AE10" s="61" t="s">
-        <v>288</v>
-      </c>
-      <c r="AF10" s="139" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="AF10" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
@@ -13913,8 +13955,8 @@
       <c r="AB14" s="117" t="s">
         <v>152</v>
       </c>
-      <c r="AC14" s="137" t="s">
-        <v>295</v>
+      <c r="AC14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="AD14" s="24"/>
       <c r="AE14" s="27"/>
@@ -14104,8 +14146,8 @@
       <c r="L19" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="M19" s="139" t="s">
-        <v>295</v>
+      <c r="M19" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="N19" s="19"/>
       <c r="O19" s="21"/>
@@ -14151,8 +14193,8 @@
       <c r="R20" s="80" t="s">
         <v>149</v>
       </c>
-      <c r="S20" s="139" t="s">
-        <v>295</v>
+      <c r="S20" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="T20" s="20"/>
       <c r="U20" s="19"/>
@@ -14331,7 +14373,7 @@
       <c r="AC24" s="19"/>
       <c r="AD24" s="19"/>
       <c r="AE24" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF24" s="41"/>
       <c r="AG24" s="5"/>
@@ -14394,7 +14436,7 @@
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
       <c r="O26" s="62" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P26" s="44" t="s">
         <v>241</v>
@@ -14554,10 +14596,10 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="125" t="s">
-        <v>288</v>
-      </c>
-      <c r="M30" s="139" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="M30" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="N30" s="19"/>
       <c r="O30" s="21"/>
@@ -14646,7 +14688,7 @@
       <c r="N32" s="19"/>
       <c r="O32" s="21"/>
       <c r="P32" s="19"/>
-      <c r="Q32" s="71" t="s">
+      <c r="Q32" s="102" t="s">
         <v>137</v>
       </c>
       <c r="R32" s="19"/>
@@ -14660,7 +14702,7 @@
       <c r="AB32" s="19"/>
       <c r="AC32" s="19"/>
       <c r="AD32" s="80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AE32" s="22"/>
       <c r="AF32" s="41"/>
@@ -14693,10 +14735,10 @@
       <c r="T33" s="35"/>
       <c r="U33" s="34"/>
       <c r="V33" s="76" t="s">
-        <v>288</v>
-      </c>
-      <c r="W33" s="154" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="W33" s="153" t="s">
+        <v>294</v>
       </c>
       <c r="X33" s="35"/>
       <c r="Y33" s="34"/>
@@ -14889,8 +14931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -16106,8 +16148,8 @@
       <c r="L32" s="20"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
-      <c r="O32" s="145" t="s">
-        <v>297</v>
+      <c r="O32" s="144" t="s">
+        <v>296</v>
       </c>
       <c r="P32" s="19"/>
       <c r="Q32" s="19"/>
@@ -17686,8 +17728,8 @@
   </sheetPr>
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -18215,8 +18257,8 @@
       <c r="K15" s="19"/>
       <c r="L15" s="20"/>
       <c r="M15" s="19"/>
-      <c r="N15" s="129" t="s">
-        <v>294</v>
+      <c r="N15" s="128" t="s">
+        <v>293</v>
       </c>
       <c r="O15" s="21"/>
       <c r="P15" s="19"/>
@@ -18237,8 +18279,8 @@
       <c r="AE15" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="AF15" s="146" t="s">
-        <v>295</v>
+      <c r="AF15" s="145" t="s">
+        <v>294</v>
       </c>
       <c r="AG15" s="5"/>
       <c r="AH15" s="5"/>
@@ -18269,8 +18311,8 @@
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
       <c r="X16" s="20"/>
-      <c r="Y16" s="129" t="s">
-        <v>297</v>
+      <c r="Y16" s="128" t="s">
+        <v>296</v>
       </c>
       <c r="Z16" s="19"/>
       <c r="AA16" s="21"/>
@@ -18718,8 +18760,8 @@
       <c r="J27" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="K27" s="139" t="s">
-        <v>295</v>
+      <c r="K27" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" s="19"/>
@@ -18819,8 +18861,8 @@
       <c r="AE29" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="AF29" s="149" t="s">
-        <v>295</v>
+      <c r="AF29" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG29" s="5"/>
       <c r="AH29" s="5"/>
@@ -19175,8 +19217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+    <sheetView topLeftCell="F18" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -19523,8 +19565,8 @@
       <c r="AE10" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="AF10" s="139" t="s">
-        <v>295</v>
+      <c r="AF10" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
@@ -19663,8 +19705,8 @@
       <c r="O14" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="P14" s="141" t="s">
-        <v>295</v>
+      <c r="P14" s="140" t="s">
+        <v>294</v>
       </c>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
@@ -19683,8 +19725,8 @@
       <c r="AA14" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="AB14" s="140" t="s">
-        <v>295</v>
+      <c r="AB14" s="139" t="s">
+        <v>294</v>
       </c>
       <c r="AC14" s="24"/>
       <c r="AD14" s="24"/>
@@ -19876,8 +19918,8 @@
       <c r="K19" s="19"/>
       <c r="L19" s="20"/>
       <c r="M19" s="19"/>
-      <c r="N19" s="129" t="s">
-        <v>178</v>
+      <c r="N19" s="80" t="s">
+        <v>184</v>
       </c>
       <c r="O19" s="21"/>
       <c r="P19" s="19"/>
@@ -20116,8 +20158,8 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="142" t="s">
-        <v>297</v>
+      <c r="H25" s="141" t="s">
+        <v>296</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -20133,8 +20175,8 @@
       <c r="T25" s="69" t="s">
         <v>187</v>
       </c>
-      <c r="U25" s="150" t="s">
-        <v>295</v>
+      <c r="U25" s="149" t="s">
+        <v>294</v>
       </c>
       <c r="V25" s="29"/>
       <c r="W25" s="29"/>
@@ -20457,8 +20499,8 @@
       <c r="H33" s="75" t="s">
         <v>252</v>
       </c>
-      <c r="I33" s="154" t="s">
-        <v>295</v>
+      <c r="I33" s="153" t="s">
+        <v>294</v>
       </c>
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
@@ -20470,8 +20512,8 @@
       <c r="Q33" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="R33" s="154" t="s">
-        <v>295</v>
+      <c r="R33" s="153" t="s">
+        <v>294</v>
       </c>
       <c r="S33" s="34"/>
       <c r="T33" s="35"/>
@@ -20672,8 +20714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView topLeftCell="F21" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -20981,8 +21023,8 @@
       <c r="H10" s="85" t="s">
         <v>255</v>
       </c>
-      <c r="I10" s="147" t="s">
-        <v>295</v>
+      <c r="I10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -20999,8 +21041,8 @@
       <c r="T10" s="86" t="s">
         <v>252</v>
       </c>
-      <c r="U10" s="147" t="s">
-        <v>295</v>
+      <c r="U10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
@@ -21202,8 +21244,8 @@
       <c r="N15" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="156" t="s">
-        <v>295</v>
+      <c r="O15" s="155" t="s">
+        <v>294</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
@@ -21220,8 +21262,8 @@
       <c r="Z15" s="80" t="s">
         <v>254</v>
       </c>
-      <c r="AA15" s="156" t="s">
-        <v>295</v>
+      <c r="AA15" s="155" t="s">
+        <v>294</v>
       </c>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -21350,7 +21392,7 @@
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
       <c r="AE18" s="81" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AF18" s="43" t="s">
         <v>217</v>
@@ -21429,8 +21471,8 @@
       <c r="Z20" s="80" t="s">
         <v>252</v>
       </c>
-      <c r="AA20" s="156" t="s">
-        <v>295</v>
+      <c r="AA20" s="155" t="s">
+        <v>294</v>
       </c>
       <c r="AB20" s="19"/>
       <c r="AC20" s="19"/>
@@ -21625,8 +21667,8 @@
       <c r="M25" s="29"/>
       <c r="N25" s="29"/>
       <c r="O25" s="31"/>
-      <c r="P25" s="136" t="s">
-        <v>301</v>
+      <c r="P25" s="135" t="s">
+        <v>300</v>
       </c>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
@@ -21767,8 +21809,8 @@
       <c r="AB28" s="19"/>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
-      <c r="AE28" s="143" t="s">
-        <v>297</v>
+      <c r="AE28" s="142" t="s">
+        <v>296</v>
       </c>
       <c r="AF28" s="5"/>
       <c r="AG28" s="5"/>
@@ -21796,11 +21838,11 @@
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
       <c r="T29" s="30"/>
-      <c r="U29" s="136" t="s">
-        <v>294</v>
+      <c r="U29" s="135" t="s">
+        <v>293</v>
       </c>
       <c r="V29" s="29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="W29" s="29"/>
       <c r="X29" s="30"/>
@@ -21829,8 +21871,8 @@
       <c r="H30" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="I30" s="139" t="s">
-        <v>295</v>
+      <c r="I30" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
@@ -22165,8 +22207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView topLeftCell="G21" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -22492,12 +22534,12 @@
       <c r="T10" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="U10" s="147" t="s">
-        <v>295</v>
+      <c r="U10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
-      <c r="X10" s="161" t="s">
+      <c r="X10" s="159" t="s">
         <v>35</v>
       </c>
       <c r="Y10" s="13"/>
@@ -22646,13 +22688,13 @@
       <c r="L14" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="M14" s="137" t="s">
-        <v>295</v>
+      <c r="M14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="26"/>
-      <c r="P14" s="135" t="s">
-        <v>299</v>
+      <c r="P14" s="134" t="s">
+        <v>298</v>
       </c>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
@@ -22660,8 +22702,8 @@
       <c r="T14" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="U14" s="137" t="s">
-        <v>295</v>
+      <c r="U14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
@@ -22838,8 +22880,8 @@
       <c r="AB18" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="AC18" s="139" t="s">
-        <v>295</v>
+      <c r="AC18" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AD18" s="19"/>
       <c r="AE18" s="22"/>
@@ -22980,16 +23022,16 @@
       <c r="L22" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="137" t="s">
-        <v>295</v>
+      <c r="M22" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="N22" s="24"/>
       <c r="O22" s="26"/>
       <c r="P22" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="Q22" s="137" t="s">
-        <v>295</v>
+      <c r="Q22" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="R22" s="24"/>
       <c r="S22" s="24"/>
@@ -23011,8 +23053,8 @@
       <c r="AC22" s="24"/>
       <c r="AD22" s="24"/>
       <c r="AE22" s="27"/>
-      <c r="AF22" s="158" t="s">
-        <v>299</v>
+      <c r="AF22" s="157" t="s">
+        <v>298</v>
       </c>
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
@@ -23139,8 +23181,8 @@
       <c r="G26" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="H26" s="134" t="s">
-        <v>299</v>
+      <c r="H26" s="133" t="s">
+        <v>298</v>
       </c>
       <c r="I26" s="24"/>
       <c r="J26" s="24"/>
@@ -23163,7 +23205,7 @@
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
-      <c r="X26" s="25" t="s">
+      <c r="X26" s="163" t="s">
         <v>46</v>
       </c>
       <c r="Y26" s="24"/>
@@ -23178,8 +23220,8 @@
       <c r="AF26" s="94" t="s">
         <v>258</v>
       </c>
-      <c r="AG26" s="148" t="s">
-        <v>295</v>
+      <c r="AG26" s="147" t="s">
+        <v>294</v>
       </c>
       <c r="AH26" s="5"/>
       <c r="AI26" s="6"/>
@@ -23320,8 +23362,8 @@
       <c r="P30" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="Q30" s="139" t="s">
-        <v>295</v>
+      <c r="Q30" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="R30" s="19"/>
       <c r="S30" s="19"/>
@@ -23478,8 +23520,8 @@
       <c r="L34" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="M34" s="157" t="s">
-        <v>295</v>
+      <c r="M34" s="156" t="s">
+        <v>294</v>
       </c>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
@@ -23492,13 +23534,13 @@
       <c r="T34" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="U34" s="157" t="s">
-        <v>295</v>
+      <c r="U34" s="156" t="s">
+        <v>294</v>
       </c>
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
-      <c r="X34" s="158" t="s">
-        <v>299</v>
+      <c r="X34" s="157" t="s">
+        <v>298</v>
       </c>
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
@@ -23644,7 +23686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="D18" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -23960,8 +24002,8 @@
       <c r="M10" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="N10" s="147" t="s">
-        <v>295</v>
+      <c r="N10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" s="13"/>
@@ -23970,8 +24012,8 @@
       <c r="S10" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="T10" s="138" t="s">
-        <v>295</v>
+      <c r="T10" s="137" t="s">
+        <v>294</v>
       </c>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -24172,8 +24214,8 @@
       <c r="N15" s="80" t="s">
         <v>252</v>
       </c>
-      <c r="O15" s="156" t="s">
-        <v>295</v>
+      <c r="O15" s="155" t="s">
+        <v>294</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
@@ -24223,8 +24265,8 @@
       <c r="X16" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="Y16" s="139" t="s">
-        <v>295</v>
+      <c r="Y16" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="Z16" s="19"/>
       <c r="AA16" s="21"/>
@@ -24402,8 +24444,8 @@
       <c r="AE20" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="AF20" s="149" t="s">
-        <v>295</v>
+      <c r="AF20" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
@@ -24484,8 +24526,8 @@
       <c r="Y22" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="Z22" s="137" t="s">
-        <v>295</v>
+      <c r="Z22" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="AA22" s="26"/>
       <c r="AB22" s="44" t="s">
@@ -24521,8 +24563,8 @@
       <c r="Q23" s="80" t="s">
         <v>252</v>
       </c>
-      <c r="R23" s="139" t="s">
-        <v>295</v>
+      <c r="R23" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="S23" s="19"/>
       <c r="T23" s="20"/>
@@ -24937,8 +24979,8 @@
       <c r="S33" s="76" t="s">
         <v>187</v>
       </c>
-      <c r="T33" s="151" t="s">
-        <v>295</v>
+      <c r="T33" s="150" t="s">
+        <v>294</v>
       </c>
       <c r="U33" s="34"/>
       <c r="V33" s="34"/>
@@ -25137,8 +25179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView topLeftCell="D19" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25449,8 +25491,8 @@
       <c r="H10" s="85" t="s">
         <v>269</v>
       </c>
-      <c r="I10" s="147" t="s">
-        <v>295</v>
+      <c r="I10" s="146" t="s">
+        <v>294</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -25841,11 +25883,11 @@
       <c r="W19" s="19"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="19"/>
-      <c r="Z19" s="129" t="s">
-        <v>296</v>
+      <c r="Z19" s="128" t="s">
+        <v>295</v>
       </c>
       <c r="AA19" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
@@ -25904,8 +25946,8 @@
       <c r="H21" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="I21" s="139" t="s">
-        <v>295</v>
+      <c r="I21" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -26216,10 +26258,10 @@
       <c r="O28" s="21"/>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
-      <c r="R28" s="80" t="s">
+      <c r="R28" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="S28" s="159"/>
+      <c r="S28" s="165"/>
       <c r="T28" s="20"/>
       <c r="U28" s="19"/>
       <c r="V28" s="19"/>
@@ -26230,8 +26272,8 @@
       <c r="AA28" s="111" t="s">
         <v>252</v>
       </c>
-      <c r="AB28" s="139" t="s">
-        <v>295</v>
+      <c r="AB28" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
@@ -26353,8 +26395,8 @@
       <c r="S31" s="19"/>
       <c r="T31" s="20"/>
       <c r="U31" s="19"/>
-      <c r="V31" s="129" t="s">
-        <v>297</v>
+      <c r="V31" s="128" t="s">
+        <v>296</v>
       </c>
       <c r="W31" s="19"/>
       <c r="X31" s="20"/>
@@ -26445,8 +26487,8 @@
       <c r="AE33" s="112" t="s">
         <v>188</v>
       </c>
-      <c r="AF33" s="149" t="s">
-        <v>295</v>
+      <c r="AF33" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG33" s="5"/>
       <c r="AH33" s="5"/>
@@ -26631,8 +26673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="O9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AI13" sqref="AI13"/>
+    <sheetView topLeftCell="C21" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0"/>
@@ -26962,8 +27004,8 @@
       <c r="Z10" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="AA10" s="152" t="s">
-        <v>295</v>
+      <c r="AA10" s="151" t="s">
+        <v>294</v>
       </c>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
@@ -26991,8 +27033,8 @@
       <c r="L11" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="139" t="s">
-        <v>295</v>
+      <c r="M11" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="N11" s="19"/>
       <c r="O11" s="21"/>
@@ -27118,8 +27160,8 @@
       <c r="P14" s="113" t="s">
         <v>144</v>
       </c>
-      <c r="Q14" s="137" t="s">
-        <v>295</v>
+      <c r="Q14" s="136" t="s">
+        <v>294</v>
       </c>
       <c r="R14" s="24"/>
       <c r="S14" s="24"/>
@@ -27222,8 +27264,8 @@
       <c r="AE16" s="81" t="s">
         <v>270</v>
       </c>
-      <c r="AF16" s="149" t="s">
-        <v>295</v>
+      <c r="AF16" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG16" s="5"/>
       <c r="AH16" s="5"/>
@@ -27291,8 +27333,8 @@
       <c r="P18" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="Q18" s="129" t="s">
-        <v>298</v>
+      <c r="Q18" s="128" t="s">
+        <v>297</v>
       </c>
       <c r="R18" s="19"/>
       <c r="S18" s="19"/>
@@ -27310,8 +27352,8 @@
       <c r="AA18" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="AB18" s="155" t="s">
-        <v>295</v>
+      <c r="AB18" s="154" t="s">
+        <v>294</v>
       </c>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
@@ -27514,8 +27556,8 @@
       <c r="Q23" s="80" t="s">
         <v>270</v>
       </c>
-      <c r="R23" s="139" t="s">
-        <v>295</v>
+      <c r="R23" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="S23" s="19"/>
       <c r="T23" s="20"/>
@@ -27562,8 +27604,8 @@
       <c r="V24" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="W24" s="139" t="s">
-        <v>295</v>
+      <c r="W24" s="138" t="s">
+        <v>294</v>
       </c>
       <c r="X24" s="20"/>
       <c r="Y24" s="19"/>
@@ -27609,8 +27651,8 @@
       <c r="AC25" s="87" t="s">
         <v>270</v>
       </c>
-      <c r="AD25" s="150" t="s">
-        <v>295</v>
+      <c r="AD25" s="149" t="s">
+        <v>294</v>
       </c>
       <c r="AE25" s="32"/>
       <c r="AF25" s="41"/>
@@ -27693,10 +27735,9 @@
       <c r="S27" s="19"/>
       <c r="T27" s="20"/>
       <c r="U27" s="19"/>
-      <c r="W27" s="80" t="s">
-        <v>264</v>
-      </c>
-      <c r="X27" s="20"/>
+      <c r="W27" s="81" t="s">
+        <v>135</v>
+      </c>
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
       <c r="AA27" s="21"/>
@@ -27905,11 +27946,11 @@
       <c r="AB32" s="19"/>
       <c r="AC32" s="19"/>
       <c r="AD32" s="19"/>
-      <c r="AE32" s="81" t="s">
-        <v>135</v>
-      </c>
-      <c r="AF32" s="149" t="s">
-        <v>295</v>
+      <c r="AE32" s="167" t="s">
+        <v>264</v>
+      </c>
+      <c r="AF32" s="148" t="s">
+        <v>294</v>
       </c>
       <c r="AG32" s="5"/>
       <c r="AH32" s="5"/>

</xml_diff>